<commit_message>
design validation single episode analysis
</commit_message>
<xml_diff>
--- a/Project Management/Updated Design Validation(v2).xlsx
+++ b/Project Management/Updated Design Validation(v2).xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27601"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_35A39EDD79B4F4689BE576C16EC03F4C46095CEC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="13545" windowHeight="12255"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13545" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DVPR Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -170,16 +174,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* \(#,##0.00\);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
-    <numFmt numFmtId="179" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* \(#,##0.00\);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
+    <numFmt numFmtId="167" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -215,159 +215,8 @@
       <name val="等线"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,194 +235,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="24">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -806,251 +469,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1058,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1066,9 +487,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1079,7 +500,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,7 +515,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1112,64 +533,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1242,6 +616,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2280,11 +1657,12 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2294,16 +1672,16 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.95" customHeight="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.33333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.875" style="1" customWidth="1"/>
-    <col min="3" max="7" width="28.4416666666667" style="1" customWidth="1"/>
+    <col min="3" max="7" width="28.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.55" customHeight="1" spans="1:7">
+    <row r="1" spans="1:7" ht="17.649999999999999" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2314,7 +1692,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" ht="7.95" customHeight="1" spans="1:7">
+    <row r="2" spans="1:7" ht="7.9" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2323,7 +1701,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" ht="15.45" customHeight="1" spans="1:7">
+    <row r="3" spans="1:7" ht="15.4" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -2340,7 +1718,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" ht="7.95" customHeight="1" spans="1:7">
+    <row r="4" spans="1:7" ht="7.9" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2349,7 +1727,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" ht="15.45" customHeight="1" spans="1:7">
+    <row r="5" spans="1:7" ht="15.4" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -2366,7 +1744,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" ht="7.95" customHeight="1" spans="1:7">
+    <row r="6" spans="1:7" ht="7.9" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2375,7 +1753,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" ht="17.55" customHeight="1" spans="1:7">
+    <row r="7" spans="1:7" ht="17.649999999999999" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -2386,7 +1764,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" ht="7.95" customHeight="1" spans="1:7">
+    <row r="8" spans="1:7" ht="7.9" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2395,7 +1773,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" ht="18.3" customHeight="1" spans="1:7">
+    <row r="9" spans="1:7" ht="18.399999999999999" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>9</v>
@@ -2416,7 +1794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="55.5" customHeight="1" spans="1:7">
+    <row r="10" spans="1:7" ht="55.5" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="16" t="s">
         <v>15</v>
@@ -2435,7 +1813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="42" customHeight="1" spans="1:7">
+    <row r="11" spans="1:7" ht="42" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="21" t="s">
         <v>19</v>
@@ -2452,7 +1830,7 @@
       <c r="F11" s="24"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" ht="57" spans="1:7">
+    <row r="12" spans="1:7" ht="57">
       <c r="A12" s="12"/>
       <c r="B12" s="21" t="s">
         <v>22</v>
@@ -2469,7 +1847,7 @@
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" ht="57" spans="1:7">
+    <row r="13" spans="1:7" ht="57">
       <c r="A13" s="12"/>
       <c r="B13" s="21" t="s">
         <v>25</v>
@@ -2486,7 +1864,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" ht="45" customHeight="1" spans="1:7">
+    <row r="14" spans="1:7" ht="45" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="21" t="s">
         <v>27</v>
@@ -2503,7 +1881,7 @@
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
     </row>
-    <row r="15" ht="45" customHeight="1" spans="1:7">
+    <row r="15" spans="1:7" ht="45" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22" t="s">
@@ -2516,7 +1894,7 @@
       <c r="F15" s="24"/>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" ht="45" customHeight="1" spans="1:7">
+    <row r="16" spans="1:7" ht="45" customHeight="1">
       <c r="A16" s="12"/>
       <c r="B16" s="21" t="s">
         <v>31</v>
@@ -2533,7 +1911,7 @@
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
     </row>
-    <row r="17" ht="45" customHeight="1" spans="1:7">
+    <row r="17" spans="1:7" ht="45" customHeight="1">
       <c r="A17" s="12"/>
       <c r="B17" s="21" t="s">
         <v>34</v>
@@ -2550,7 +1928,7 @@
       <c r="F17" s="24"/>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" ht="55.05" customHeight="1" spans="1:7">
+    <row r="18" spans="1:7" ht="55.15" customHeight="1">
       <c r="A18" s="12"/>
       <c r="B18" s="21" t="s">
         <v>36</v>
@@ -2567,7 +1945,7 @@
       <c r="F18" s="24"/>
       <c r="G18" s="25"/>
     </row>
-    <row r="19" ht="45" customHeight="1" spans="1:7">
+    <row r="19" spans="1:7" ht="45" customHeight="1">
       <c r="A19" s="12"/>
       <c r="B19" s="21" t="s">
         <v>38</v>
@@ -2584,7 +1962,7 @@
       <c r="F19" s="24"/>
       <c r="G19" s="25"/>
     </row>
-    <row r="20" ht="45" customHeight="1" spans="1:7">
+    <row r="20" spans="1:7" ht="45" customHeight="1">
       <c r="A20" s="12"/>
       <c r="B20" s="21" t="s">
         <v>40</v>
@@ -2601,7 +1979,7 @@
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" ht="55.05" customHeight="1" spans="1:7">
+    <row r="21" spans="1:7" ht="55.15" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" s="21" t="s">
         <v>42</v>
@@ -2618,7 +1996,7 @@
       <c r="F21" s="24"/>
       <c r="G21" s="25"/>
     </row>
-    <row r="22" ht="55.05" customHeight="1" spans="1:7">
+    <row r="22" spans="1:7" ht="55.15" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="21" t="s">
         <v>44</v>
@@ -2635,7 +2013,7 @@
       <c r="F22" s="24"/>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" ht="45" customHeight="1" spans="1:7">
+    <row r="23" spans="1:7" ht="45" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" s="26"/>
       <c r="C23" s="24"/>
@@ -2644,7 +2022,7 @@
       <c r="F23" s="24"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" ht="45" customHeight="1" spans="1:7">
+    <row r="24" spans="1:7" ht="45" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="26"/>
       <c r="C24" s="24"/>
@@ -2653,7 +2031,7 @@
       <c r="F24" s="24"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" ht="45" customHeight="1" spans="1:7">
+    <row r="25" spans="1:7" ht="45" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="26"/>
       <c r="C25" s="24"/>
@@ -2662,7 +2040,7 @@
       <c r="F25" s="24"/>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" ht="45" customHeight="1" spans="1:7">
+    <row r="26" spans="1:7" ht="45" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -2673,7 +2051,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" scale="77" orientation="landscape"/>
+  <pageSetup scale="77" orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>